<commit_message>
Recomputed test results for task 4. Replaced unrecognized characters in test documents.
</commit_message>
<xml_diff>
--- a/resources/MP1_TESTING_GLOBAL_MASTER.xlsx
+++ b/resources/MP1_TESTING_GLOBAL_MASTER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7jlap\Documents\UBC\Year 2\CPEN 221\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962D2074-EC59-42F1-9455-9826894A5038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E16A19-D85D-4BBA-8994-C94C036B3A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1037,7 +1037,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AZ988"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
@@ -47987,8 +47987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F075131B-D00A-44B9-8747-F6F7FB30D6E9}">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -48091,7 +48091,7 @@
       </c>
       <c r="O3">
         <f t="shared" si="4"/>
-        <v>1.4499999999999993</v>
+        <v>1.2537499999999966</v>
       </c>
       <c r="P3">
         <f t="shared" si="5"/>
@@ -48186,7 +48186,7 @@
       </c>
       <c r="O6" s="4">
         <f>SUM(O1:O5)+50*Sheet1!U174</f>
-        <v>47.773135914997845</v>
+        <v>47.576885914997845</v>
       </c>
       <c r="P6" s="4">
         <f>SUM(P1:P5)+50*Sheet1!V174</f>
@@ -48270,7 +48270,7 @@
       </c>
       <c r="O9">
         <f t="shared" si="9"/>
-        <v>2.1765000000000008</v>
+        <v>1.9802499999999981</v>
       </c>
       <c r="P9">
         <f t="shared" si="10"/>
@@ -48344,7 +48344,7 @@
       </c>
       <c r="O12" s="4">
         <f>SUM(O7:O11)+50*Sheet1!Y174</f>
-        <v>59.611018283286015</v>
+        <v>59.414768283286008</v>
       </c>
       <c r="P12" s="4">
         <f>SUM(P7:P11)+50*Sheet1!Z174</f>
@@ -48416,7 +48416,7 @@
       </c>
       <c r="O15">
         <f t="shared" si="13"/>
-        <v>1.7600000000000016</v>
+        <v>1.5637499999999989</v>
       </c>
       <c r="P15">
         <f t="shared" si="14"/>
@@ -48478,7 +48478,7 @@
       </c>
       <c r="O18" s="4">
         <f>SUM(O13:O17)+50*Sheet1!AB174</f>
-        <v>52.206928904167675</v>
+        <v>52.010678904167676</v>
       </c>
       <c r="P18" s="4">
         <f>SUM(P13:P17)+50*Sheet1!AC174</f>
@@ -48538,7 +48538,7 @@
       </c>
       <c r="O21">
         <f t="shared" si="16"/>
-        <v>1.110000000000003</v>
+        <v>0.91375000000000028</v>
       </c>
       <c r="P21">
         <f t="shared" si="17"/>
@@ -48588,7 +48588,7 @@
     <row r="24" spans="1:16">
       <c r="O24" s="4">
         <f>SUM(O19:O23)+50*Sheet1!AD174</f>
-        <v>50.294270332003109</v>
+        <v>50.098020332003102</v>
       </c>
       <c r="P24" s="4">
         <f>SUM(P19:P23)+50*Sheet1!AE174</f>
@@ -48632,15 +48632,15 @@
         <v>213</v>
       </c>
       <c r="F27">
-        <v>4.0979999999999999</v>
+        <v>4.1372499999999999</v>
       </c>
       <c r="J27">
         <f t="shared" si="18"/>
-        <v>20.49</v>
+        <v>20.686250000000001</v>
       </c>
       <c r="P27">
         <f t="shared" si="19"/>
-        <v>3.5499999999995424E-2</v>
+        <v>0.23174999999999812</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -48678,7 +48678,7 @@
     <row r="30" spans="1:16">
       <c r="P30" s="4">
         <f>SUM(P25:P29)+50*Sheet1!AF174</f>
-        <v>51.995191722684325</v>
+        <v>52.191441722684324</v>
       </c>
     </row>
     <row r="31" spans="1:16">

</xml_diff>